<commit_message>
Mejora Carga Monitor y Campo
</commit_message>
<xml_diff>
--- a/Parlo Banco Falabella Marzo 2023.xlsx
+++ b/Parlo Banco Falabella Marzo 2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nelson/Documents/REACT/evaluacion3/Proyecto-Evaluacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7E0515-39CB-E341-AD26-5EE41B154ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BFE57E7-7EC3-7845-9E66-782B8B140812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24980" windowHeight="15040" xr2:uid="{71602248-84B9-4F52-AF12-48A334590F43}"/>
+    <workbookView xWindow="4860" yWindow="2740" windowWidth="24980" windowHeight="15040" xr2:uid="{71602248-84B9-4F52-AF12-48A334590F43}"/>
   </bookViews>
   <sheets>
     <sheet name="Parlo Ejemplo" sheetId="2" r:id="rId1"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="102">
   <si>
     <t>FILA</t>
   </si>
@@ -391,12 +391,6 @@
   </si>
   <si>
     <t>id</t>
-  </si>
-  <si>
-    <t>Matías Erazo</t>
-  </si>
-  <si>
-    <t>Juan Rojas</t>
   </si>
 </sst>
 </file>
@@ -2287,7 +2281,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Listas"/>
@@ -2670,8 +2664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81148EFC-B3D6-5E49-96A3-91B77DF397D9}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3183,7 +3177,7 @@
         <v>36</v>
       </c>
       <c r="N10" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="O10" t="s">
         <v>36</v>
@@ -3333,7 +3327,7 @@
         <v>28</v>
       </c>
       <c r="N13" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="O13" t="s">
         <v>30</v>
@@ -3433,7 +3427,7 @@
         <v>28</v>
       </c>
       <c r="N15" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="O15" t="s">
         <v>30</v>
@@ -3533,7 +3527,7 @@
         <v>28</v>
       </c>
       <c r="N17" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="O17" t="s">
         <v>73</v>
@@ -3683,7 +3677,7 @@
         <v>36</v>
       </c>
       <c r="N20" t="s">
-        <v>103</v>
+        <v>29</v>
       </c>
       <c r="O20" t="s">
         <v>36</v>
@@ -3733,7 +3727,7 @@
         <v>28</v>
       </c>
       <c r="N21" t="s">
-        <v>103</v>
+        <v>29</v>
       </c>
       <c r="O21" t="s">
         <v>39</v>

</xml_diff>